<commit_message>
Database utils for Sql server
</commit_message>
<xml_diff>
--- a/SeleniumCSharpSpecflowProject/ScenarioLevelTestData.xlsx
+++ b/SeleniumCSharpSpecflowProject/ScenarioLevelTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yash\Documents\Projects\SeleniumSpecFlow\SeleniumSpecFlow\SeleniumCSharpSpecflowProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4591DA3-8566-41BF-A512-D8847D5C996A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835272F0-51C4-4065-883A-B0D255452AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Login to the application with the newly created user and Delete the newly created user</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Yashwanth</t>
+  </si>
+  <si>
+    <t>Arul</t>
   </si>
 </sst>
 </file>
@@ -389,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,9 +413,11 @@
     <col min="2" max="2" width="35" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +430,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -430,8 +450,14 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -439,7 +465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>